<commit_message>
add example file modified
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -9,6 +9,41 @@
     <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">oui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jamais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hasard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bonjour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vous</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -339,7 +374,354 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C2" t="n">
+        <v>21</v>
+      </c>
+      <c r="D2" t="n">
+        <v>31</v>
+      </c>
+      <c r="E2" t="n">
+        <v>41</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2" t="n">
+        <v>60</v>
+      </c>
+      <c r="H2" t="n">
+        <v>70</v>
+      </c>
+      <c r="I2" t="n">
+        <v>80</v>
+      </c>
+      <c r="J2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3" t="n">
+        <v>22</v>
+      </c>
+      <c r="D3" t="n">
+        <v>32</v>
+      </c>
+      <c r="E3" t="n">
+        <v>42</v>
+      </c>
+      <c r="F3" t="n">
+        <v>51</v>
+      </c>
+      <c r="G3" t="n">
+        <v>61</v>
+      </c>
+      <c r="H3" t="n">
+        <v>71</v>
+      </c>
+      <c r="I3" t="n">
+        <v>81</v>
+      </c>
+      <c r="J3" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>13</v>
+      </c>
+      <c r="C4" t="n">
+        <v>23</v>
+      </c>
+      <c r="D4" t="n">
+        <v>33</v>
+      </c>
+      <c r="E4" t="n">
+        <v>43</v>
+      </c>
+      <c r="F4" t="n">
+        <v>52</v>
+      </c>
+      <c r="G4" t="n">
+        <v>62</v>
+      </c>
+      <c r="H4" t="n">
+        <v>72</v>
+      </c>
+      <c r="I4" t="n">
+        <v>82</v>
+      </c>
+      <c r="J4" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>14</v>
+      </c>
+      <c r="C5" t="n">
+        <v>24</v>
+      </c>
+      <c r="D5" t="n">
+        <v>34</v>
+      </c>
+      <c r="E5" t="n">
+        <v>44</v>
+      </c>
+      <c r="F5" t="n">
+        <v>53</v>
+      </c>
+      <c r="G5" t="n">
+        <v>63</v>
+      </c>
+      <c r="H5" t="n">
+        <v>73</v>
+      </c>
+      <c r="I5" t="n">
+        <v>83</v>
+      </c>
+      <c r="J5" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>15</v>
+      </c>
+      <c r="C6" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>35</v>
+      </c>
+      <c r="E6" t="n">
+        <v>45</v>
+      </c>
+      <c r="F6" t="n">
+        <v>54</v>
+      </c>
+      <c r="G6" t="n">
+        <v>64</v>
+      </c>
+      <c r="H6" t="n">
+        <v>74</v>
+      </c>
+      <c r="I6" t="n">
+        <v>84</v>
+      </c>
+      <c r="J6" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>16</v>
+      </c>
+      <c r="C7" t="n">
+        <v>26</v>
+      </c>
+      <c r="D7" t="n">
+        <v>36</v>
+      </c>
+      <c r="E7" t="n">
+        <v>46</v>
+      </c>
+      <c r="F7" t="n">
+        <v>55</v>
+      </c>
+      <c r="G7" t="n">
+        <v>65</v>
+      </c>
+      <c r="H7" t="n">
+        <v>75</v>
+      </c>
+      <c r="I7" t="n">
+        <v>85</v>
+      </c>
+      <c r="J7" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>17</v>
+      </c>
+      <c r="C8" t="n">
+        <v>27</v>
+      </c>
+      <c r="D8" t="n">
+        <v>37</v>
+      </c>
+      <c r="E8" t="n">
+        <v>47</v>
+      </c>
+      <c r="F8" t="n">
+        <v>56</v>
+      </c>
+      <c r="G8" t="n">
+        <v>66</v>
+      </c>
+      <c r="H8" t="n">
+        <v>76</v>
+      </c>
+      <c r="I8" t="n">
+        <v>86</v>
+      </c>
+      <c r="J8" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>18</v>
+      </c>
+      <c r="C9" t="n">
+        <v>28</v>
+      </c>
+      <c r="D9" t="n">
+        <v>38</v>
+      </c>
+      <c r="E9" t="n">
+        <v>48</v>
+      </c>
+      <c r="F9" t="n">
+        <v>57</v>
+      </c>
+      <c r="G9" t="n">
+        <v>67</v>
+      </c>
+      <c r="H9" t="n">
+        <v>77</v>
+      </c>
+      <c r="I9" t="n">
+        <v>87</v>
+      </c>
+      <c r="J9" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>19</v>
+      </c>
+      <c r="C10" t="n">
+        <v>29</v>
+      </c>
+      <c r="D10" t="n">
+        <v>39</v>
+      </c>
+      <c r="E10" t="n">
+        <v>49</v>
+      </c>
+      <c r="F10" t="n">
+        <v>58</v>
+      </c>
+      <c r="G10" t="n">
+        <v>68</v>
+      </c>
+      <c r="H10" t="n">
+        <v>78</v>
+      </c>
+      <c r="I10" t="n">
+        <v>88</v>
+      </c>
+      <c r="J10" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20</v>
+      </c>
+      <c r="C11" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" t="n">
+        <v>40</v>
+      </c>
+      <c r="E11" t="n">
+        <v>50</v>
+      </c>
+      <c r="F11" t="n">
+        <v>59</v>
+      </c>
+      <c r="G11" t="n">
+        <v>69</v>
+      </c>
+      <c r="H11" t="n">
+        <v>79</v>
+      </c>
+      <c r="I11" t="n">
+        <v>89</v>
+      </c>
+      <c r="J11" t="n">
         <v>99</v>
       </c>
     </row>

</xml_diff>